<commit_message>
added docs to readme
</commit_message>
<xml_diff>
--- a/Project Planning Spreadsheet.xlsx
+++ b/Project Planning Spreadsheet.xlsx
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DG113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,7 +1908,7 @@
         <v>34</v>
       </c>
       <c r="I16" s="21">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J16" s="6">
         <v>1</v>
@@ -1982,7 +1982,7 @@
         <v>34</v>
       </c>
       <c r="I17" s="21">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J17" s="6">
         <v>2</v>
@@ -2056,7 +2056,7 @@
         <v>34</v>
       </c>
       <c r="I18" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="6">
         <v>2</v>
@@ -2130,7 +2130,7 @@
         <v>34</v>
       </c>
       <c r="I19" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="6">
         <v>1</v>
@@ -2204,7 +2204,7 @@
         <v>34</v>
       </c>
       <c r="I20" s="21">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J20" s="6">
         <v>4</v>
@@ -2278,7 +2278,7 @@
         <v>34</v>
       </c>
       <c r="I21" s="21">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J21" s="6">
         <v>8</v>

</xml_diff>